<commit_message>
Calculating sums of multiple .xlsx
</commit_message>
<xml_diff>
--- a/Excel & Data tables/ExcelTestData.xlsx
+++ b/Excel & Data tables/ExcelTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JacobRozsa\Documents\UiPath\Foundations Training\Excel &amp; Data tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5E1271-4C17-491F-93B8-E56545C7945F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99B6D36-E85E-4B2D-AA31-0B2E0B7EF05B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,22 @@
     <t>City</t>
   </si>
   <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Boise</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
     <t>Jake</t>
   </si>
   <si>
     <t>Bubba</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Boise</t>
-  </si>
-  <si>
-    <t>Allen</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,24 +390,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>